<commit_message>
Add side effect first option and doc
</commit_message>
<xml_diff>
--- a/samples/sample-ci/analysis/ci-logs.xlsx
+++ b/samples/sample-ci/analysis/ci-logs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matts966/alphasql/samples/sample-ci/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matts966/ghq/github.com/Matts966/alphasql/samples/sample-ci/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ABE3B2-B108-CD4E-A594-4D0E11D15B6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EC2C52-67F9-5F4E-9E64-FF17034C3490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{1C410683-E4EA-1443-97E8-543CE771AAB0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1C410683-E4EA-1443-97E8-543CE771AAB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -163,7 +163,7 @@
           <c:strCache>
             <c:ptCount val="2"/>
             <c:pt idx="0">
-              <c:v>827</c:v>
+              <c:v>1445</c:v>
             </c:pt>
             <c:pt idx="1">
               <c:v>RESULTS ON CI</c:v>
@@ -663,7 +663,11 @@
                     <a:fld id="{01C675FB-20DE-7B4A-818D-5BF482ED94FE}" type="CATEGORYNAME">
                       <a:rPr lang="en-US" altLang="ja-JP" sz="1200"/>
                       <a:pPr>
-                        <a:defRPr sz="1200"/>
+                        <a:defRPr sz="1200">
+                          <a:solidFill>
+                            <a:schemeClr val="accent1"/>
+                          </a:solidFill>
+                        </a:defRPr>
                       </a:pPr>
                       <a:t>[分類名]</a:t>
                     </a:fld>
@@ -687,7 +691,7 @@
                   <a:pPr>
                     <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent6"/>
+                        <a:schemeClr val="accent1"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -967,19 +971,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>584</c:v>
+                  <c:v>1106</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96</c:v>
+                  <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -1975,7 +1979,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1988,7 +1992,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>584</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1996,7 +2000,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2004,7 +2008,11 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>96</v>
+        <v>142</v>
+      </c>
+      <c r="C4">
+        <f>SUM(B4:B8)</f>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2012,7 +2020,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2020,7 +2028,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2045,7 +2053,7 @@
       </c>
       <c r="B10">
         <f>SUM(B1:B8)</f>
-        <v>827</v>
+        <v>1445</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>

</xml_diff>